<commit_message>
Edits on current outline
</commit_message>
<xml_diff>
--- a/notes/freezexp_muoutput_manual.xlsx
+++ b/notes/freezexp_muoutput_manual.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/chillfreeze/analyses/output/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D16904-7E8E-5341-88E8-1CEFCAD916E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28028"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19500" yWindow="460" windowWidth="29360" windowHeight="19520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12120" yWindow="5840" windowWidth="34040" windowHeight="19520"/>
   </bookViews>
   <sheets>
     <sheet name="freezexp_cat" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="74">
   <si>
     <t>DVR</t>
   </si>
@@ -176,14 +175,80 @@
     <t>ACESAC and BETPAP had increased root growth but CORRAC had decresed root growth - all for 90%</t>
   </si>
   <si>
-    <t>CORRAC had decreased root growth for 50%</t>
+    <t>tough</t>
+  </si>
+  <si>
+    <t>root:shoot</t>
+  </si>
+  <si>
+    <t>dvr</t>
+  </si>
+  <si>
+    <t>htdiff</t>
+  </si>
+  <si>
+    <t>meristem</t>
+  </si>
+  <si>
+    <t>Treatment effects were common across phenology and leaf traits, but marginal for growth traits (height, biomass RS) and no effect on gslength</t>
+  </si>
+  <si>
+    <t>treat</t>
+  </si>
+  <si>
+    <t>There was generally little effect of 6 weeks of chilling</t>
+  </si>
+  <si>
+    <t>There WAS an effect of 8 weeks of chilling.</t>
+  </si>
+  <si>
+    <t>There is at best mrginal interactions -- save for GS length.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 out of 8 </t>
+  </si>
+  <si>
+    <t>3 out of 8</t>
+  </si>
+  <si>
+    <t>1 out of 8</t>
+  </si>
+  <si>
+    <t>4 out of 6</t>
+  </si>
+  <si>
+    <t>6 out of 8</t>
+  </si>
+  <si>
+    <t>There is at best mrginal interactions -- save for htdiff -- but this varied by species.</t>
+  </si>
+  <si>
+    <t>phenology</t>
+  </si>
+  <si>
+    <t>growth</t>
+  </si>
+  <si>
+    <t>leaves</t>
+  </si>
+  <si>
+    <t>8wk chill and tx impact DVR; there are some predictable but understable gs effects (so these should be subordinate)</t>
+  </si>
+  <si>
+    <t>tx damages meristem with marginal effects on growth, there are some marginal chill effects</t>
+  </si>
+  <si>
+    <t>tx changes leaves! Chilling also does. Interestingly toughness goes down across chill and tx … why? (I would naively expect the opposite)</t>
+  </si>
+  <si>
+    <t>*Side note -- make sure this lines up with supp … it seems like the models differ (e.g., there's shoot growth in the supp but no root to shoot).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -325,8 +390,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -506,8 +587,32 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -622,8 +727,140 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -666,12 +903,91 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="92">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -700,11 +1016,61 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -771,7 +1137,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -823,7 +1189,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1017,23 +1383,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="5" max="5" width="40.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1053,7 +1422,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1067,7 +1436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1081,7 +1450,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1098,7 +1467,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1112,7 +1481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1125,8 +1494,35 @@
       <c r="D6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I6" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q6" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1142,8 +1538,38 @@
       <c r="E7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I7" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="O7" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="P7" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="R7" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1156,8 +1582,38 @@
       <c r="D8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="O8" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="P8" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="R8" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1173,8 +1629,38 @@
       <c r="E9" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I9" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="O9" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="P9" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q9" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="R9" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1187,8 +1673,38 @@
       <c r="D10" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I10" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="M10" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="N10" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="R10" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1204,8 +1720,38 @@
       <c r="E11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I11" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="N11" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="O11" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="P11" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="R11" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1224,8 +1770,38 @@
       <c r="F12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I12" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="R12" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1238,8 +1814,38 @@
       <c r="D13" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I13" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R13" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1255,8 +1861,38 @@
       <c r="F14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I14" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="R14" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1272,8 +1908,38 @@
       <c r="E15" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I15" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="P15" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="R15" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1289,8 +1955,38 @@
       <c r="F16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I16" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="P16" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="R16" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1307,7 +2003,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1323,8 +2019,14 @@
       <c r="E18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J18" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="K18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -1340,8 +2042,14 @@
       <c r="E19" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J19" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="K19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -1354,8 +2062,14 @@
       <c r="D20" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J20" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="K20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -1369,7 +2083,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1382,8 +2096,11 @@
       <c r="D22" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1403,7 +2120,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -1423,7 +2140,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1437,7 +2154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1451,7 +2168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1468,7 +2185,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1485,7 +2202,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -1502,7 +2219,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -1519,7 +2236,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -1533,7 +2250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -1547,7 +2264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -1561,7 +2278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -1578,7 +2295,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -1592,7 +2309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -1606,7 +2323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -1626,7 +2343,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -1640,7 +2357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>46</v>
       </c>
@@ -1657,7 +2374,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -1674,7 +2391,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -1687,51 +2404,59 @@
       <c r="D41" t="s">
         <v>3</v>
       </c>
-      <c r="E41" t="s">
-        <v>51</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>